<commit_message>
update fs19c metadata with treatment group
</commit_message>
<xml_diff>
--- a/Files/FS19C_metadata.xlsx
+++ b/Files/FS19C_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathy.mou/Desktop/FS19/FS19C/FS19C_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathy.mou/Desktop/Notebook/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4217903A-CFEE-4643-ACF7-470FEB7075E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871B1D6A-3AEB-7D4A-9C77-607649A500EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="1720" windowWidth="22860" windowHeight="16440" xr2:uid="{7ABC44E6-C22C-6344-8A46-31B7B878C723}"/>
+    <workbookView xWindow="1320" yWindow="640" windowWidth="28300" windowHeight="19420" xr2:uid="{7ABC44E6-C22C-6344-8A46-31B7B878C723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="310">
   <si>
     <t>Sample_Name</t>
   </si>
@@ -940,6 +940,21 @@
   </si>
   <si>
     <t>96 - 441 FE C t=1</t>
+  </si>
+  <si>
+    <t>EDL933</t>
+  </si>
+  <si>
+    <t>TW14588</t>
+  </si>
+  <si>
+    <t>RM6067</t>
+  </si>
+  <si>
+    <t>FRIK1989</t>
+  </si>
+  <si>
+    <t>FS19 Group</t>
   </si>
 </sst>
 </file>
@@ -947,7 +962,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1000,7 +1015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1315,10 +1330,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DDB985-620C-A842-AD44-54CB7E7C3DE5}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1335,7 +1351,7 @@
     <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,8 +1382,11 @@
       <c r="J1" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1398,8 +1417,11 @@
       <c r="J2" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K2" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1430,8 +1452,11 @@
       <c r="J3" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K3" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1462,8 +1487,11 @@
       <c r="J4" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K4" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1494,8 +1522,11 @@
       <c r="J5" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K5" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1526,8 +1557,11 @@
       <c r="J6" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K6" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1558,8 +1592,11 @@
       <c r="J7" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K7" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1590,8 +1627,11 @@
       <c r="J8" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K8" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1622,8 +1662,11 @@
       <c r="J9" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K9" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -1654,8 +1697,11 @@
       <c r="J10" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K10" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1686,8 +1732,11 @@
       <c r="J11" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K11" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1718,8 +1767,11 @@
       <c r="J12" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K12" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -1750,8 +1802,11 @@
       <c r="J13" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K13" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -1782,8 +1837,11 @@
       <c r="J14" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K14" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1814,8 +1872,11 @@
       <c r="J15" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K15" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -1846,8 +1907,11 @@
       <c r="J16" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K16" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1878,8 +1942,11 @@
       <c r="J17" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K17" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -1910,8 +1977,11 @@
       <c r="J18" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K18" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>43</v>
       </c>
@@ -1942,8 +2012,11 @@
       <c r="J19" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K19" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1974,8 +2047,11 @@
       <c r="J20" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K20" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
@@ -2006,8 +2082,11 @@
       <c r="J21" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K21" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
@@ -2038,8 +2117,11 @@
       <c r="J22" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K22" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>51</v>
       </c>
@@ -2070,8 +2152,11 @@
       <c r="J23" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K23" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -2102,8 +2187,11 @@
       <c r="J24" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K24" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
@@ -2134,8 +2222,11 @@
       <c r="J25" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K25" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>57</v>
       </c>
@@ -2166,8 +2257,11 @@
       <c r="J26" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K26" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>59</v>
       </c>
@@ -2198,8 +2292,11 @@
       <c r="J27" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K27" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>61</v>
       </c>
@@ -2230,8 +2327,11 @@
       <c r="J28" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K28" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>63</v>
       </c>
@@ -2262,8 +2362,11 @@
       <c r="J29" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K29" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -2294,8 +2397,11 @@
       <c r="J30" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K30" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>67</v>
       </c>
@@ -2326,8 +2432,11 @@
       <c r="J31" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K31" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
@@ -2358,8 +2467,11 @@
       <c r="J32" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K32" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>71</v>
       </c>
@@ -2390,8 +2502,11 @@
       <c r="J33" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K33" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>73</v>
       </c>
@@ -2422,8 +2537,11 @@
       <c r="J34" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K34" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>75</v>
       </c>
@@ -2454,8 +2572,11 @@
       <c r="J35" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K35" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>77</v>
       </c>
@@ -2486,8 +2607,11 @@
       <c r="J36" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K36" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>79</v>
       </c>
@@ -2518,8 +2642,11 @@
       <c r="J37" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K37" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>81</v>
       </c>
@@ -2550,8 +2677,11 @@
       <c r="J38" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K38" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>83</v>
       </c>
@@ -2582,8 +2712,11 @@
       <c r="J39" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K39" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>85</v>
       </c>
@@ -2614,8 +2747,11 @@
       <c r="J40" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K40" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
@@ -2646,8 +2782,11 @@
       <c r="J41" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K41" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>89</v>
       </c>
@@ -2678,8 +2817,11 @@
       <c r="J42" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K42" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
@@ -2710,8 +2852,11 @@
       <c r="J43" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K43" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>93</v>
       </c>
@@ -2742,8 +2887,11 @@
       <c r="J44" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K44" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>95</v>
       </c>
@@ -2774,8 +2922,11 @@
       <c r="J45" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K45" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>97</v>
       </c>
@@ -2806,8 +2957,11 @@
       <c r="J46" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K46" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>99</v>
       </c>
@@ -2838,8 +2992,11 @@
       <c r="J47" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K47" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>101</v>
       </c>
@@ -2870,8 +3027,11 @@
       <c r="J48" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K48" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>103</v>
       </c>
@@ -2902,8 +3062,11 @@
       <c r="J49" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K49" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>105</v>
       </c>
@@ -2934,8 +3097,11 @@
       <c r="J50" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K50" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>107</v>
       </c>
@@ -2966,8 +3132,11 @@
       <c r="J51" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K51" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>109</v>
       </c>
@@ -2998,8 +3167,11 @@
       <c r="J52" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K52" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>111</v>
       </c>
@@ -3030,8 +3202,11 @@
       <c r="J53" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K53" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>113</v>
       </c>
@@ -3062,8 +3237,11 @@
       <c r="J54" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K54" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>115</v>
       </c>
@@ -3094,8 +3272,11 @@
       <c r="J55" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K55" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>117</v>
       </c>
@@ -3126,8 +3307,11 @@
       <c r="J56" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K56" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>119</v>
       </c>
@@ -3158,8 +3342,11 @@
       <c r="J57" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K57" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>121</v>
       </c>
@@ -3190,8 +3377,11 @@
       <c r="J58" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K58" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>123</v>
       </c>
@@ -3222,8 +3412,11 @@
       <c r="J59" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K59" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>125</v>
       </c>
@@ -3254,8 +3447,11 @@
       <c r="J60" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K60" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>127</v>
       </c>
@@ -3286,8 +3482,11 @@
       <c r="J61" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K61" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>129</v>
       </c>
@@ -3318,8 +3517,11 @@
       <c r="J62" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K62" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>131</v>
       </c>
@@ -3350,8 +3552,11 @@
       <c r="J63" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K63" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>133</v>
       </c>
@@ -3382,8 +3587,11 @@
       <c r="J64" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K64" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>135</v>
       </c>
@@ -3414,8 +3622,11 @@
       <c r="J65" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K65" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>137</v>
       </c>
@@ -3446,8 +3657,11 @@
       <c r="J66" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K66" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>139</v>
       </c>
@@ -3478,8 +3692,11 @@
       <c r="J67" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K67" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>141</v>
       </c>
@@ -3510,8 +3727,11 @@
       <c r="J68" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K68" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>143</v>
       </c>
@@ -3542,8 +3762,11 @@
       <c r="J69" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K69" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>145</v>
       </c>
@@ -3574,8 +3797,11 @@
       <c r="J70" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K70" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>147</v>
       </c>
@@ -3606,8 +3832,11 @@
       <c r="J71" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K71" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>149</v>
       </c>
@@ -3638,8 +3867,11 @@
       <c r="J72" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K72" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>151</v>
       </c>
@@ -3670,8 +3902,11 @@
       <c r="J73" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K73" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>153</v>
       </c>
@@ -3702,8 +3937,11 @@
       <c r="J74" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K74" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>155</v>
       </c>
@@ -3734,8 +3972,11 @@
       <c r="J75" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K75" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>157</v>
       </c>
@@ -3766,8 +4007,11 @@
       <c r="J76" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K76" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>159</v>
       </c>
@@ -3798,8 +4042,11 @@
       <c r="J77" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K77" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>161</v>
       </c>
@@ -3830,8 +4077,11 @@
       <c r="J78" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K78" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>163</v>
       </c>
@@ -3862,8 +4112,11 @@
       <c r="J79" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K79" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>165</v>
       </c>
@@ -3894,8 +4147,11 @@
       <c r="J80" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K80" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>167</v>
       </c>
@@ -3926,8 +4182,11 @@
       <c r="J81" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K81" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>169</v>
       </c>
@@ -3958,8 +4217,11 @@
       <c r="J82" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K82" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>171</v>
       </c>
@@ -3990,8 +4252,11 @@
       <c r="J83" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K83" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>173</v>
       </c>
@@ -4022,8 +4287,11 @@
       <c r="J84" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K84" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>175</v>
       </c>
@@ -4054,8 +4322,11 @@
       <c r="J85" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K85" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>177</v>
       </c>
@@ -4086,8 +4357,11 @@
       <c r="J86" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K86" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>179</v>
       </c>
@@ -4118,8 +4392,11 @@
       <c r="J87" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K87" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>181</v>
       </c>
@@ -4150,8 +4427,11 @@
       <c r="J88" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K88" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>183</v>
       </c>
@@ -4182,8 +4462,11 @@
       <c r="J89" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K89" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>185</v>
       </c>
@@ -4214,8 +4497,11 @@
       <c r="J90" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K90" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>187</v>
       </c>
@@ -4246,8 +4532,11 @@
       <c r="J91" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K91" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>189</v>
       </c>
@@ -4278,8 +4567,11 @@
       <c r="J92" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K92" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>191</v>
       </c>
@@ -4310,8 +4602,11 @@
       <c r="J93" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K93" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>193</v>
       </c>
@@ -4342,8 +4637,11 @@
       <c r="J94" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K94" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>195</v>
       </c>
@@ -4374,8 +4672,11 @@
       <c r="J95" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K95" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>197</v>
       </c>
@@ -4406,8 +4707,11 @@
       <c r="J96" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K96" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>199</v>
       </c>
@@ -4437,6 +4741,9 @@
       </c>
       <c r="J97" s="1" t="s">
         <v>208</v>
+      </c>
+      <c r="K97" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>